<commit_message>
Docs - Dodanie Metryk biznesowych.
</commit_message>
<xml_diff>
--- a/adl/Metryki.xlsx
+++ b/adl/Metryki.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\MgService\adl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F206E6DA-CFC8-425A-979B-67D1F0682885}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43AFB94E-11F2-4028-8AFD-E646A9459EBA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="27">
   <si>
     <t>Testowalność</t>
   </si>
@@ -84,13 +84,43 @@
   </si>
   <si>
     <t>n.d</t>
+  </si>
+  <si>
+    <t>Metryki architektoniczne</t>
+  </si>
+  <si>
+    <t>Metryki biznesowe</t>
+  </si>
+  <si>
+    <t>Czas dodania wpisu dziennika</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Czas w sekunadach potrzebny na dodanie nowego wpisu dziennika</t>
+  </si>
+  <si>
+    <t>Czas dodania klienta wraz z pojazdem</t>
+  </si>
+  <si>
+    <t>Czas dodania standardowej naprawy</t>
+  </si>
+  <si>
+    <t>Czas w sekunadach potrzebny na dodanie nowego klienta wraz z pojazdem</t>
+  </si>
+  <si>
+    <t>Czas w sekunadach potrzebny na dodanie standardowej naprawy</t>
+  </si>
+  <si>
+    <t>Metryka weryfikująca sukces</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,8 +153,40 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -141,6 +203,11 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -151,12 +218,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -165,9 +233,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="9" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Dobry" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutralny" xfId="3" builtinId="28"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
     <cellStyle name="Zły" xfId="2" builtinId="27"/>
   </cellStyles>
@@ -447,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:H6"/>
+  <dimension ref="A2:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,98 +531,215 @@
     <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.85546875" customWidth="1"/>
-    <col min="4" max="4" width="62" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.140625" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+    </row>
+    <row r="4" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>0</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E5" s="4">
         <v>0</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F5" s="1">
         <v>0.5</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G5" s="1">
         <v>0.75</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H5" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E6" s="3">
         <v>1</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <v>1</v>
       </c>
-      <c r="G5">
+      <c r="G6">
         <v>0</v>
       </c>
-      <c r="H5">
+      <c r="H6">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>